<commit_message>
Please check the read me file.
Please check the read me file for all file details and comments.
</commit_message>
<xml_diff>
--- a/contributions/enam_shaikh_23440037/cluster_file.xlsx
+++ b/contributions/enam_shaikh_23440037/cluster_file.xlsx
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -887,7 +887,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -1447,7 +1447,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
@@ -1587,7 +1587,7 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -1727,7 +1727,7 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2077,7 +2077,7 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49">
@@ -2147,7 +2147,7 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
@@ -2287,7 +2287,7 @@
         </is>
       </c>
       <c r="G53" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55">
@@ -2357,7 +2357,7 @@
         </is>
       </c>
       <c r="G55" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="G56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="G59" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
@@ -2532,7 +2532,7 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
@@ -2567,7 +2567,7 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62">
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63">
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64">
@@ -2672,7 +2672,7 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -2707,7 +2707,7 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67">
@@ -2777,7 +2777,7 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68">
@@ -2812,7 +2812,7 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="G69" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73">
@@ -2987,7 +2987,7 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75">
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="G75" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -3127,7 +3127,7 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
@@ -3162,7 +3162,7 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79">
@@ -3197,7 +3197,7 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="G80" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -3337,7 +3337,7 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85">
@@ -3407,7 +3407,7 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -3477,7 +3477,7 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3547,7 +3547,7 @@
         </is>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3617,7 +3617,7 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3652,7 +3652,7 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
@@ -3687,7 +3687,7 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -3722,7 +3722,7 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
@@ -3792,7 +3792,7 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97">
@@ -3827,7 +3827,7 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98">
@@ -3862,7 +3862,7 @@
         </is>
       </c>
       <c r="G98" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -3897,7 +3897,7 @@
         </is>
       </c>
       <c r="G99" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101">
@@ -3967,7 +3967,7 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
@@ -4037,7 +4037,7 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104">
@@ -4072,7 +4072,7 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -4107,7 +4107,7 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
@@ -4142,7 +4142,7 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -4177,7 +4177,7 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -4212,7 +4212,7 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -4247,7 +4247,7 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110">
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111">
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112">
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113">
@@ -4387,7 +4387,7 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115">
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="G115" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116">
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="G116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4527,7 +4527,7 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118">
@@ -4562,7 +4562,7 @@
         </is>
       </c>
       <c r="G118" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119">
@@ -4597,7 +4597,7 @@
         </is>
       </c>
       <c r="G119" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
@@ -4667,7 +4667,7 @@
         </is>
       </c>
       <c r="G121" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122">
@@ -4702,7 +4702,7 @@
         </is>
       </c>
       <c r="G122" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123">
@@ -4737,7 +4737,7 @@
         </is>
       </c>
       <c r="G123" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124">
@@ -4772,7 +4772,7 @@
         </is>
       </c>
       <c r="G124" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125">
@@ -4807,7 +4807,7 @@
         </is>
       </c>
       <c r="G125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="G126" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127">
@@ -4877,7 +4877,7 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128">
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129">
@@ -4947,7 +4947,7 @@
         </is>
       </c>
       <c r="G129" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130">
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="G130" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131">
@@ -5017,7 +5017,7 @@
         </is>
       </c>
       <c r="G131" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
@@ -5052,7 +5052,7 @@
         </is>
       </c>
       <c r="G132" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133">
@@ -5087,7 +5087,7 @@
         </is>
       </c>
       <c r="G133" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134">
@@ -5122,7 +5122,7 @@
         </is>
       </c>
       <c r="G134" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135">
@@ -5157,7 +5157,7 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136">
@@ -5192,7 +5192,7 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137">
@@ -5227,7 +5227,7 @@
         </is>
       </c>
       <c r="G137" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138">
@@ -5262,7 +5262,7 @@
         </is>
       </c>
       <c r="G138" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -5297,7 +5297,7 @@
         </is>
       </c>
       <c r="G139" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140">
@@ -5332,7 +5332,7 @@
         </is>
       </c>
       <c r="G140" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141">
@@ -5367,7 +5367,7 @@
         </is>
       </c>
       <c r="G141" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -5402,7 +5402,7 @@
         </is>
       </c>
       <c r="G142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -5437,7 +5437,7 @@
         </is>
       </c>
       <c r="G143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="G144" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145">
@@ -5507,7 +5507,7 @@
         </is>
       </c>
       <c r="G145" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146">
@@ -5542,7 +5542,7 @@
         </is>
       </c>
       <c r="G146" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147">
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148">
@@ -5612,7 +5612,7 @@
         </is>
       </c>
       <c r="G148" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149">
@@ -5647,7 +5647,7 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -5682,7 +5682,7 @@
         </is>
       </c>
       <c r="G150" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151">
@@ -5717,7 +5717,7 @@
         </is>
       </c>
       <c r="G151" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152">
@@ -5752,7 +5752,7 @@
         </is>
       </c>
       <c r="G152" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153">
@@ -5787,7 +5787,7 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154">
@@ -5822,7 +5822,7 @@
         </is>
       </c>
       <c r="G154" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -5857,7 +5857,7 @@
         </is>
       </c>
       <c r="G155" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -5892,7 +5892,7 @@
         </is>
       </c>
       <c r="G156" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="157">
@@ -5927,7 +5927,7 @@
         </is>
       </c>
       <c r="G157" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158">
@@ -5962,7 +5962,7 @@
         </is>
       </c>
       <c r="G158" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159">
@@ -5997,7 +5997,7 @@
         </is>
       </c>
       <c r="G159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -6032,7 +6032,7 @@
         </is>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -6067,7 +6067,7 @@
         </is>
       </c>
       <c r="G161" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162">
@@ -6102,7 +6102,7 @@
         </is>
       </c>
       <c r="G162" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -6137,7 +6137,7 @@
         </is>
       </c>
       <c r="G163" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -6172,7 +6172,7 @@
         </is>
       </c>
       <c r="G164" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -6207,7 +6207,7 @@
         </is>
       </c>
       <c r="G165" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166">
@@ -6242,7 +6242,7 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167">
@@ -6277,7 +6277,7 @@
         </is>
       </c>
       <c r="G167" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -6312,7 +6312,7 @@
         </is>
       </c>
       <c r="G168" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
@@ -6347,7 +6347,7 @@
         </is>
       </c>
       <c r="G169" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -6382,7 +6382,7 @@
         </is>
       </c>
       <c r="G170" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -6417,7 +6417,7 @@
         </is>
       </c>
       <c r="G171" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -6452,7 +6452,7 @@
         </is>
       </c>
       <c r="G172" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -6487,7 +6487,7 @@
         </is>
       </c>
       <c r="G173" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -6522,7 +6522,7 @@
         </is>
       </c>
       <c r="G174" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -6557,7 +6557,7 @@
         </is>
       </c>
       <c r="G175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -6592,7 +6592,7 @@
         </is>
       </c>
       <c r="G176" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177">
@@ -6627,7 +6627,7 @@
         </is>
       </c>
       <c r="G177" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178">
@@ -6662,7 +6662,7 @@
         </is>
       </c>
       <c r="G178" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179">
@@ -6697,7 +6697,7 @@
         </is>
       </c>
       <c r="G179" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180">
@@ -6732,7 +6732,7 @@
         </is>
       </c>
       <c r="G180" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -6767,7 +6767,7 @@
         </is>
       </c>
       <c r="G181" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="182">
@@ -6802,7 +6802,7 @@
         </is>
       </c>
       <c r="G182" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183">
@@ -6837,7 +6837,7 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184">
@@ -6872,7 +6872,7 @@
         </is>
       </c>
       <c r="G184" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185">
@@ -6907,7 +6907,7 @@
         </is>
       </c>
       <c r="G185" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="186">
@@ -6942,7 +6942,7 @@
         </is>
       </c>
       <c r="G186" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -6977,7 +6977,7 @@
         </is>
       </c>
       <c r="G187" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188">
@@ -7012,7 +7012,7 @@
         </is>
       </c>
       <c r="G188" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189">
@@ -7047,7 +7047,7 @@
         </is>
       </c>
       <c r="G189" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -7082,7 +7082,7 @@
         </is>
       </c>
       <c r="G190" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191">
@@ -7117,7 +7117,7 @@
         </is>
       </c>
       <c r="G191" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192">
@@ -7152,7 +7152,7 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193">
@@ -7187,7 +7187,7 @@
         </is>
       </c>
       <c r="G193" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="194">
@@ -7222,7 +7222,7 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -7257,7 +7257,7 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -7292,7 +7292,7 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -7327,7 +7327,7 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198">
@@ -7362,7 +7362,7 @@
         </is>
       </c>
       <c r="G198" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -7397,7 +7397,7 @@
         </is>
       </c>
       <c r="G199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -7432,7 +7432,7 @@
         </is>
       </c>
       <c r="G200" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -7467,7 +7467,7 @@
         </is>
       </c>
       <c r="G201" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="202">
@@ -7502,7 +7502,7 @@
         </is>
       </c>
       <c r="G202" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203">
@@ -7537,7 +7537,7 @@
         </is>
       </c>
       <c r="G203" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -7572,7 +7572,7 @@
         </is>
       </c>
       <c r="G204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
@@ -7607,7 +7607,7 @@
         </is>
       </c>
       <c r="G205" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="206">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="G206" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207">
@@ -7677,7 +7677,7 @@
         </is>
       </c>
       <c r="G207" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="208">
@@ -7712,7 +7712,7 @@
         </is>
       </c>
       <c r="G208" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -7747,7 +7747,7 @@
         </is>
       </c>
       <c r="G209" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="210">
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="G210" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211">
@@ -7817,7 +7817,7 @@
         </is>
       </c>
       <c r="G211" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212">
@@ -7852,7 +7852,7 @@
         </is>
       </c>
       <c r="G212" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="213">
@@ -7887,7 +7887,7 @@
         </is>
       </c>
       <c r="G213" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="214">
@@ -7922,7 +7922,7 @@
         </is>
       </c>
       <c r="G214" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="215">
@@ -7957,7 +7957,7 @@
         </is>
       </c>
       <c r="G215" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="216">
@@ -7992,7 +7992,7 @@
         </is>
       </c>
       <c r="G216" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217">
@@ -8027,7 +8027,7 @@
         </is>
       </c>
       <c r="G217" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="218">
@@ -8062,7 +8062,7 @@
         </is>
       </c>
       <c r="G218" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219">
@@ -8097,7 +8097,7 @@
         </is>
       </c>
       <c r="G219" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -8132,7 +8132,7 @@
         </is>
       </c>
       <c r="G220" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="G221" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="222">
@@ -8202,7 +8202,7 @@
         </is>
       </c>
       <c r="G222" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -8237,7 +8237,7 @@
         </is>
       </c>
       <c r="G223" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="224">
@@ -8272,7 +8272,7 @@
         </is>
       </c>
       <c r="G224" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225">
@@ -8307,7 +8307,7 @@
         </is>
       </c>
       <c r="G225" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="226">
@@ -8342,7 +8342,7 @@
         </is>
       </c>
       <c r="G226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -8377,7 +8377,7 @@
         </is>
       </c>
       <c r="G227" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -8412,7 +8412,7 @@
         </is>
       </c>
       <c r="G228" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -8447,7 +8447,7 @@
         </is>
       </c>
       <c r="G229" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="230">
@@ -8482,7 +8482,7 @@
         </is>
       </c>
       <c r="G230" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="231">
@@ -8517,7 +8517,7 @@
         </is>
       </c>
       <c r="G231" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="232">
@@ -8552,7 +8552,7 @@
         </is>
       </c>
       <c r="G232" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233">
@@ -8587,7 +8587,7 @@
         </is>
       </c>
       <c r="G233" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234">
@@ -8622,7 +8622,7 @@
         </is>
       </c>
       <c r="G234" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="235">
@@ -8657,7 +8657,7 @@
         </is>
       </c>
       <c r="G235" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="236">
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="G236" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="237">
@@ -8727,7 +8727,7 @@
         </is>
       </c>
       <c r="G237" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="238">
@@ -8762,7 +8762,7 @@
         </is>
       </c>
       <c r="G238" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239">
@@ -8797,7 +8797,7 @@
         </is>
       </c>
       <c r="G239" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240">
@@ -8832,7 +8832,7 @@
         </is>
       </c>
       <c r="G240" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="241">
@@ -8867,7 +8867,7 @@
         </is>
       </c>
       <c r="G241" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="242">
@@ -8902,7 +8902,7 @@
         </is>
       </c>
       <c r="G242" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -8937,7 +8937,7 @@
         </is>
       </c>
       <c r="G243" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="244">
@@ -8972,7 +8972,7 @@
         </is>
       </c>
       <c r="G244" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="245">
@@ -9007,7 +9007,7 @@
         </is>
       </c>
       <c r="G245" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="246">
@@ -9042,7 +9042,7 @@
         </is>
       </c>
       <c r="G246" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247">
@@ -9077,7 +9077,7 @@
         </is>
       </c>
       <c r="G247" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="248">
@@ -9112,7 +9112,7 @@
         </is>
       </c>
       <c r="G248" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="249">
@@ -9147,7 +9147,7 @@
         </is>
       </c>
       <c r="G249" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -9182,7 +9182,7 @@
         </is>
       </c>
       <c r="G250" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="251">
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="G251" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="252">
@@ -9252,7 +9252,7 @@
         </is>
       </c>
       <c r="G252" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="253">
@@ -9287,7 +9287,7 @@
         </is>
       </c>
       <c r="G253" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254">
@@ -9322,7 +9322,7 @@
         </is>
       </c>
       <c r="G254" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="255">
@@ -9357,7 +9357,7 @@
         </is>
       </c>
       <c r="G255" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="256">
@@ -9392,7 +9392,7 @@
         </is>
       </c>
       <c r="G256" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
@@ -9427,7 +9427,7 @@
         </is>
       </c>
       <c r="G257" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="258">
@@ -9462,7 +9462,7 @@
         </is>
       </c>
       <c r="G258" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="259">
@@ -9497,7 +9497,7 @@
         </is>
       </c>
       <c r="G259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260">
@@ -9532,7 +9532,7 @@
         </is>
       </c>
       <c r="G260" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="261">
@@ -9567,7 +9567,7 @@
         </is>
       </c>
       <c r="G261" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
@@ -9602,7 +9602,7 @@
         </is>
       </c>
       <c r="G262" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
@@ -9637,7 +9637,7 @@
         </is>
       </c>
       <c r="G263" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="264">
@@ -9672,7 +9672,7 @@
         </is>
       </c>
       <c r="G264" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="265">
@@ -9707,7 +9707,7 @@
         </is>
       </c>
       <c r="G265" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -9742,7 +9742,7 @@
         </is>
       </c>
       <c r="G266" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -9777,7 +9777,7 @@
         </is>
       </c>
       <c r="G267" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
@@ -9812,7 +9812,7 @@
         </is>
       </c>
       <c r="G268" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -9882,7 +9882,7 @@
         </is>
       </c>
       <c r="G270" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="271">
@@ -9917,7 +9917,7 @@
         </is>
       </c>
       <c r="G271" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="272">
@@ -9952,7 +9952,7 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273">
@@ -9987,7 +9987,7 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="274">
@@ -10022,7 +10022,7 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275">
@@ -10057,7 +10057,7 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276">
@@ -10092,7 +10092,7 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="277">
@@ -10127,7 +10127,7 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278">
@@ -10162,7 +10162,7 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279">
@@ -10197,7 +10197,7 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="280">
@@ -10232,7 +10232,7 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="281">
@@ -10267,7 +10267,7 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="282">
@@ -10302,7 +10302,7 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283">
@@ -10337,7 +10337,7 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="284">
@@ -10372,7 +10372,7 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="285">
@@ -10407,7 +10407,7 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="286">
@@ -10442,7 +10442,7 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287">
@@ -10477,7 +10477,7 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="288">
@@ -10512,7 +10512,7 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289">
@@ -10547,7 +10547,7 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290">
@@ -10582,7 +10582,7 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291">
@@ -10617,7 +10617,7 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="292">
@@ -10652,7 +10652,7 @@
         </is>
       </c>
       <c r="G292" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="293">
@@ -10687,7 +10687,7 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="294">
@@ -10722,7 +10722,7 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295">
@@ -10757,7 +10757,7 @@
         </is>
       </c>
       <c r="G295" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">
@@ -10792,7 +10792,7 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297">
@@ -10827,7 +10827,7 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298">
@@ -10862,7 +10862,7 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="299">
@@ -10897,7 +10897,7 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="300">
@@ -10932,7 +10932,7 @@
         </is>
       </c>
       <c r="G300" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301">
@@ -10967,7 +10967,7 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="302">
@@ -11002,7 +11002,7 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="303">
@@ -11037,7 +11037,7 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="304">
@@ -11072,7 +11072,7 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305">
@@ -11107,7 +11107,7 @@
         </is>
       </c>
       <c r="G305" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="306">
@@ -11142,7 +11142,7 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307">
@@ -11177,7 +11177,7 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="308">
@@ -11212,7 +11212,7 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309">
@@ -11247,7 +11247,7 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310">
@@ -11282,7 +11282,7 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311">
@@ -11317,7 +11317,7 @@
         </is>
       </c>
       <c r="G311" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="312">
@@ -11352,7 +11352,7 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="313">
@@ -11387,7 +11387,7 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="314">
@@ -11422,7 +11422,7 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="315">
@@ -11457,7 +11457,7 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="316">
@@ -11492,7 +11492,7 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="317">
@@ -11527,7 +11527,7 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318">
@@ -11562,7 +11562,7 @@
         </is>
       </c>
       <c r="G318" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="319">
@@ -11597,7 +11597,7 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="320">
@@ -11632,7 +11632,7 @@
         </is>
       </c>
       <c r="G320" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321">
@@ -11667,7 +11667,7 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="322">
@@ -11702,7 +11702,7 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="323">
@@ -11737,7 +11737,7 @@
         </is>
       </c>
       <c r="G323" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="324">
@@ -11772,7 +11772,7 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="325">
@@ -11807,7 +11807,7 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="326">
@@ -11842,7 +11842,7 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327">
@@ -11877,7 +11877,7 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328">
@@ -11912,7 +11912,7 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329">
@@ -11947,7 +11947,7 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330">
@@ -11982,7 +11982,7 @@
         </is>
       </c>
       <c r="G330" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="331">
@@ -12017,7 +12017,7 @@
         </is>
       </c>
       <c r="G331" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332">
@@ -12052,7 +12052,7 @@
         </is>
       </c>
       <c r="G332" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="333">
@@ -12087,7 +12087,7 @@
         </is>
       </c>
       <c r="G333" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334">
@@ -12122,7 +12122,7 @@
         </is>
       </c>
       <c r="G334" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335">
@@ -12157,7 +12157,7 @@
         </is>
       </c>
       <c r="G335" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="336">
@@ -12192,7 +12192,7 @@
         </is>
       </c>
       <c r="G336" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="337">
@@ -12227,7 +12227,7 @@
         </is>
       </c>
       <c r="G337" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="338">
@@ -12262,7 +12262,7 @@
         </is>
       </c>
       <c r="G338" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="339">
@@ -12297,7 +12297,7 @@
         </is>
       </c>
       <c r="G339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340">
@@ -12332,7 +12332,7 @@
         </is>
       </c>
       <c r="G340" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="341">
@@ -12367,7 +12367,7 @@
         </is>
       </c>
       <c r="G341" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="342">
@@ -12402,7 +12402,7 @@
         </is>
       </c>
       <c r="G342" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="343">
@@ -12437,7 +12437,7 @@
         </is>
       </c>
       <c r="G343" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="344">
@@ -12472,7 +12472,7 @@
         </is>
       </c>
       <c r="G344" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="345">
@@ -12507,7 +12507,7 @@
         </is>
       </c>
       <c r="G345" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346">
@@ -12542,7 +12542,7 @@
         </is>
       </c>
       <c r="G346" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="347">
@@ -12577,7 +12577,7 @@
         </is>
       </c>
       <c r="G347" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="348">
@@ -12612,7 +12612,7 @@
         </is>
       </c>
       <c r="G348" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349">
@@ -12647,7 +12647,7 @@
         </is>
       </c>
       <c r="G349" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350">
@@ -12682,7 +12682,7 @@
         </is>
       </c>
       <c r="G350" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="351">
@@ -12717,7 +12717,7 @@
         </is>
       </c>
       <c r="G351" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="352">
@@ -12787,7 +12787,7 @@
         </is>
       </c>
       <c r="G353" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="354">
@@ -12822,7 +12822,7 @@
         </is>
       </c>
       <c r="G354" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="355">
@@ -12857,7 +12857,7 @@
         </is>
       </c>
       <c r="G355" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="356">
@@ -12892,7 +12892,7 @@
         </is>
       </c>
       <c r="G356" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357">
@@ -12927,7 +12927,7 @@
         </is>
       </c>
       <c r="G357" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="358">
@@ -12962,7 +12962,7 @@
         </is>
       </c>
       <c r="G358" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359">
@@ -12997,7 +12997,7 @@
         </is>
       </c>
       <c r="G359" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="360">
@@ -13032,7 +13032,7 @@
         </is>
       </c>
       <c r="G360" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="361">
@@ -13067,7 +13067,7 @@
         </is>
       </c>
       <c r="G361" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362">
@@ -13102,7 +13102,7 @@
         </is>
       </c>
       <c r="G362" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363">
@@ -13137,7 +13137,7 @@
         </is>
       </c>
       <c r="G363" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364">
@@ -13172,7 +13172,7 @@
         </is>
       </c>
       <c r="G364" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="365">
@@ -13207,7 +13207,7 @@
         </is>
       </c>
       <c r="G365" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="366">
@@ -13242,7 +13242,7 @@
         </is>
       </c>
       <c r="G366" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="367">
@@ -13277,7 +13277,7 @@
         </is>
       </c>
       <c r="G367" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="368">
@@ -13312,7 +13312,7 @@
         </is>
       </c>
       <c r="G368" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369">
@@ -13347,7 +13347,7 @@
         </is>
       </c>
       <c r="G369" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="370">
@@ -13382,7 +13382,7 @@
         </is>
       </c>
       <c r="G370" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="371">
@@ -13417,7 +13417,7 @@
         </is>
       </c>
       <c r="G371" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="372">
@@ -13452,7 +13452,7 @@
         </is>
       </c>
       <c r="G372" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="373">
@@ -13487,7 +13487,7 @@
         </is>
       </c>
       <c r="G373" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="374">
@@ -13522,7 +13522,7 @@
         </is>
       </c>
       <c r="G374" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="375">
@@ -13557,7 +13557,7 @@
         </is>
       </c>
       <c r="G375" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="376">
@@ -13592,7 +13592,7 @@
         </is>
       </c>
       <c r="G376" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="377">
@@ -13627,7 +13627,7 @@
         </is>
       </c>
       <c r="G377" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="378">
@@ -13662,7 +13662,7 @@
         </is>
       </c>
       <c r="G378" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="379">
@@ -13697,7 +13697,7 @@
         </is>
       </c>
       <c r="G379" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="380">
@@ -13732,7 +13732,7 @@
         </is>
       </c>
       <c r="G380" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381">
@@ -13767,7 +13767,7 @@
         </is>
       </c>
       <c r="G381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
@@ -13802,7 +13802,7 @@
         </is>
       </c>
       <c r="G382" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="383">
@@ -13837,7 +13837,7 @@
         </is>
       </c>
       <c r="G383" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="384">
@@ -13872,7 +13872,7 @@
         </is>
       </c>
       <c r="G384" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="385">
@@ -13907,7 +13907,7 @@
         </is>
       </c>
       <c r="G385" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="386">
@@ -13942,7 +13942,7 @@
         </is>
       </c>
       <c r="G386" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="387">
@@ -13977,7 +13977,7 @@
         </is>
       </c>
       <c r="G387" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="388">
@@ -14012,7 +14012,7 @@
         </is>
       </c>
       <c r="G388" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="389">
@@ -14047,7 +14047,7 @@
         </is>
       </c>
       <c r="G389" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390">
@@ -14082,7 +14082,7 @@
         </is>
       </c>
       <c r="G390" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="391">
@@ -14117,7 +14117,7 @@
         </is>
       </c>
       <c r="G391" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392">
@@ -14152,7 +14152,7 @@
         </is>
       </c>
       <c r="G392" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="393">
@@ -14187,7 +14187,7 @@
         </is>
       </c>
       <c r="G393" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="394">
@@ -14222,7 +14222,7 @@
         </is>
       </c>
       <c r="G394" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="395">
@@ -14257,7 +14257,7 @@
         </is>
       </c>
       <c r="G395" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="396">
@@ -14292,7 +14292,7 @@
         </is>
       </c>
       <c r="G396" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="397">
@@ -14327,7 +14327,7 @@
         </is>
       </c>
       <c r="G397" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="398">
@@ -14362,7 +14362,7 @@
         </is>
       </c>
       <c r="G398" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="399">
@@ -14397,7 +14397,7 @@
         </is>
       </c>
       <c r="G399" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400">
@@ -14432,7 +14432,7 @@
         </is>
       </c>
       <c r="G400" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="401">
@@ -14467,7 +14467,7 @@
         </is>
       </c>
       <c r="G401" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="402">
@@ -14502,7 +14502,7 @@
         </is>
       </c>
       <c r="G402" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="403">
@@ -14537,7 +14537,7 @@
         </is>
       </c>
       <c r="G403" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="404">
@@ -14572,7 +14572,7 @@
         </is>
       </c>
       <c r="G404" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405">
@@ -14607,7 +14607,7 @@
         </is>
       </c>
       <c r="G405" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="406">
@@ -14642,7 +14642,7 @@
         </is>
       </c>
       <c r="G406" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="407">
@@ -14677,7 +14677,7 @@
         </is>
       </c>
       <c r="G407" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="408">
@@ -14712,7 +14712,7 @@
         </is>
       </c>
       <c r="G408" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="409">
@@ -14747,7 +14747,7 @@
         </is>
       </c>
       <c r="G409" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410">
@@ -14782,7 +14782,7 @@
         </is>
       </c>
       <c r="G410" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="411">
@@ -14817,7 +14817,7 @@
         </is>
       </c>
       <c r="G411" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="412">
@@ -14852,7 +14852,7 @@
         </is>
       </c>
       <c r="G412" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="413">
@@ -14887,7 +14887,7 @@
         </is>
       </c>
       <c r="G413" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="414">
@@ -14922,7 +14922,7 @@
         </is>
       </c>
       <c r="G414" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="415">
@@ -14957,7 +14957,7 @@
         </is>
       </c>
       <c r="G415" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="416">
@@ -14992,7 +14992,7 @@
         </is>
       </c>
       <c r="G416" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="417">
@@ -15027,7 +15027,7 @@
         </is>
       </c>
       <c r="G417" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>